<commit_message>
Issue #73: Standardize title-cased values to lowercase
</commit_message>
<xml_diff>
--- a/data/clean_data.xlsx
+++ b/data/clean_data.xlsx
@@ -228,7 +228,7 @@
     <t xml:space="preserve">Male</t>
   </si>
   <si>
-    <t xml:space="preserve">Adult</t>
+    <t xml:space="preserve">adult</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;1</t>
@@ -252,7 +252,7 @@
     <t xml:space="preserve">A03</t>
   </si>
   <si>
-    <t xml:space="preserve">Subadult</t>
+    <t xml:space="preserve">subadult</t>
   </si>
   <si>
     <t xml:space="preserve">20.5</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">A77</t>
   </si>
   <si>
-    <t xml:space="preserve">Fawn</t>
+    <t xml:space="preserve">fawn</t>
   </si>
   <si>
     <t xml:space="preserve">4.8262992562333604</t>

</xml_diff>

<commit_message>
Standardize also the 'Sex' and 'Detected' labels
</commit_message>
<xml_diff>
--- a/data/clean_data.xlsx
+++ b/data/clean_data.xlsx
@@ -225,7 +225,7 @@
     <t xml:space="preserve">C. elaphus</t>
   </si>
   <si>
-    <t xml:space="preserve">Male</t>
+    <t xml:space="preserve">male</t>
   </si>
   <si>
     <t xml:space="preserve">adult</t>
@@ -273,7 +273,7 @@
     <t xml:space="preserve">A07</t>
   </si>
   <si>
-    <t xml:space="preserve">Female</t>
+    <t xml:space="preserve">female</t>
   </si>
   <si>
     <t xml:space="preserve">42.6</t>

</xml_diff>